<commit_message>
update 20160329 - 42, 20160329 - 43
</commit_message>
<xml_diff>
--- a/20160329 - 042/running_logs/logs.xlsx
+++ b/20160329 - 042/running_logs/logs.xlsx
@@ -142,12 +142,13 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:I10"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.246963562753"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -188,6 +189,7 @@
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>